<commit_message>
Change some variables for running
</commit_message>
<xml_diff>
--- a/data_collection.xlsx
+++ b/data_collection.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A91CC2B-FC44-4326-8C32-1DFFAD6CF008}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4620125-426F-4140-975F-5562E4F12552}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="5813" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -14,7 +14,6 @@
     <sheet name="Sup_Fig_5_fasted_lactate" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -6823,7 +6822,7 @@
   <dimension ref="A1:DT66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="DK12" sqref="DK12"/>
+      <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>